<commit_message>
In progress: automatic control
</commit_message>
<xml_diff>
--- a/src_python/gui.xlsx
+++ b/src_python/gui.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\_GitHub_repo\project-Humidistat\src_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC6BFDA-1BAB-4562-B1C1-F8D6CFDAB26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4ACCF66-0E8F-44B0-B5D9-B7EB11CAC7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8784" yWindow="3936" windowWidth="21192" windowHeight="14100" xr2:uid="{1B013C4B-837A-43D6-8AC9-8C59D25C2F9D}"/>
+    <workbookView xWindow="30612" yWindow="4356" windowWidth="20376" windowHeight="12360" xr2:uid="{1B013C4B-837A-43D6-8AC9-8C59D25C2F9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>ON/OFF</t>
   </si>
@@ -54,47 +54,125 @@
     <t>Load  config</t>
   </si>
   <si>
-    <t>H_1 LO</t>
-  </si>
-  <si>
-    <t>H_1 HI</t>
-  </si>
-  <si>
-    <t>H_2 LO</t>
-  </si>
-  <si>
-    <t>H_2 HI</t>
-  </si>
-  <si>
     <t>valve 1</t>
   </si>
   <si>
-    <t>Auto thresholds:</t>
-  </si>
-  <si>
-    <t>Auto actuators:</t>
-  </si>
-  <si>
-    <t>H_1 &lt; LO</t>
-  </si>
-  <si>
-    <t>H_1 &gt; HI</t>
-  </si>
-  <si>
-    <t>H_2 &lt; LO</t>
-  </si>
-  <si>
-    <t>H_2 &gt; HI</t>
-  </si>
-  <si>
     <t>Idea: valve 1 is connected to water reservoir and bubble pump to increase humidity. Valve 2 is connected to very low flow nitrogen line to reduce humidity</t>
+  </si>
+  <si>
+    <t>Setpoint</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>incr RH</t>
+  </si>
+  <si>
+    <t>decr RH</t>
+  </si>
+  <si>
+    <t>burst length</t>
+  </si>
+  <si>
+    <t>Actuator setup:</t>
+  </si>
+  <si>
+    <t>delta LO</t>
+  </si>
+  <si>
+    <t>delta HI</t>
+  </si>
+  <si>
+    <t>Coarse controller: Quickly reach new setpoint when far away</t>
+  </si>
+  <si>
+    <t>Fine controller: Maintain setpoint in short-burst mode</t>
+  </si>
+  <si>
+    <t>The coarse controller will be in effect when the humidity reading is outside of the `FINE CONTROL` bandwidth based around the desired setpoint.</t>
+  </si>
+  <si>
+    <t>The `FINE CONTROL` bandwidth is defined by `delta LO` and `delta HI` below and above the desired setpoint.</t>
+  </si>
+  <si>
+    <t>The fine controller will be in effect when the humidity reading is within the `FINE CONTROL` bandwidth, i.e. near the desired setpoint.</t>
+  </si>
+  <si>
+    <t>Coarse control will engage the actuators continuously until the reading lies within the `FINE CONTROL` bandwidth.</t>
+  </si>
+  <si>
+    <t>Fine control will periodically check the humidity reading and engage the actuators for a short time period, called a burst,</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>NOTE: Should be larger than the response time of the system on a single burst</t>
+  </si>
+  <si>
+    <t>update period</t>
+  </si>
+  <si>
+    <t>NOTE: The burst length should be large enough for the system to see a noticeable effect, but small enough to enable fine control. Say, -0.3 to -0.5 % RH.</t>
+  </si>
+  <si>
+    <t>NOTE: The burst length should be large enough for the system to see a noticeable effect, but small enough to enable fine control. Say, +0.3 to +0.5 % RH.</t>
+  </si>
+  <si>
+    <t>burst incr RH</t>
+  </si>
+  <si>
+    <t>burst decr RH</t>
+  </si>
+  <si>
+    <t>auto controller</t>
+  </si>
+  <si>
+    <t>COARSE/FINE/DEAD</t>
+  </si>
+  <si>
+    <t>toggle</t>
+  </si>
+  <si>
+    <t>pushb</t>
+  </si>
+  <si>
+    <t>indicator</t>
+  </si>
+  <si>
+    <t>The `DEADBAND` bandwidth is the smallest region around the setpoint where, if the reading is inside of it, no actuators will be engaged.</t>
+  </si>
+  <si>
+    <t>DEADBAND</t>
+  </si>
+  <si>
+    <t>whenever the reading is within the `FINE CONTROL` bandwidth but outside of the smaller `DEADBAND` bandwidth.</t>
+  </si>
+  <si>
+    <t>actuators_incr_RH</t>
+  </si>
+  <si>
+    <t>actuators_decr_RH</t>
+  </si>
+  <si>
+    <t>feedback_on_sensor_no</t>
+  </si>
+  <si>
+    <t>-2</t>
+  </si>
+  <si>
+    <t>NOTE: negative</t>
+  </si>
+  <si>
+    <t>NOTE: positive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,8 +190,17 @@
     </font>
     <font>
       <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -136,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -185,11 +272,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -200,20 +300,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -221,14 +318,29 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -251,18 +363,6 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
@@ -276,11 +376,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -291,36 +391,27 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>68580</xdr:colOff>
-          <xdr:row>16</xdr:row>
+          <xdr:row>22</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>731520</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="662940" cy="228600"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Check Box 1" hidden="1">
+            <xdr:cNvPr id="1040" name="Check Box 16" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
+                  <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{906EC5AE-BDA7-461F-A345-D7207FEFB4FB}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -379,34 +470,29 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>68580</xdr:colOff>
-          <xdr:row>17</xdr:row>
+          <xdr:row>23</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>731520</xdr:colOff>
-          <xdr:row>19</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="662940" cy="228600"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1026" name="Check Box 2" hidden="1">
+            <xdr:cNvPr id="1041" name="Check Box 17" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1026"/>
+                  <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E2DA661-D708-4D2F-886A-17BC155D655B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -465,34 +551,29 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>68580</xdr:colOff>
-          <xdr:row>18</xdr:row>
+          <xdr:row>24</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>731520</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="662940" cy="228600"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1027" name="Check Box 3" hidden="1">
+            <xdr:cNvPr id="1042" name="Check Box 18" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1027"/>
+                  <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F529280B-B6D3-4EC4-BB96-31B01FC8214C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -551,34 +632,29 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>2</xdr:col>
+          <xdr:col>4</xdr:col>
           <xdr:colOff>68580</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>22</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>731520</xdr:colOff>
-          <xdr:row>21</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="662940" cy="228600"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1028" name="Check Box 4" hidden="1">
+            <xdr:cNvPr id="1043" name="Check Box 19" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1028"/>
+                  <a14:compatExt spid="_x0000_s1043"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BFD846C-497C-45B5-A97B-55C4A855A698}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -637,34 +713,29 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>2</xdr:col>
+          <xdr:col>4</xdr:col>
           <xdr:colOff>68580</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>23</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>731520</xdr:colOff>
-          <xdr:row>22</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="662940" cy="228600"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1029" name="Check Box 5" hidden="1">
+            <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1029"/>
+                  <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDDA1C7F-E4CB-4D5E-A5A5-6C845957CDF3}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -723,34 +794,29 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>2</xdr:col>
+          <xdr:col>4</xdr:col>
           <xdr:colOff>68580</xdr:colOff>
-          <xdr:row>21</xdr:row>
+          <xdr:row>24</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>731520</xdr:colOff>
-          <xdr:row>23</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="662940" cy="228600"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1030" name="Check Box 6" hidden="1">
+            <xdr:cNvPr id="1045" name="Check Box 21" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1030"/>
+                  <a14:compatExt spid="_x0000_s1045"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF9361BD-BF2E-4929-AD70-D8DA630174A1}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -809,7 +875,7 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -817,21 +883,21 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>4</xdr:col>
+          <xdr:col>2</xdr:col>
           <xdr:colOff>68580</xdr:colOff>
-          <xdr:row>16</xdr:row>
+          <xdr:row>27</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:ext cx="662940" cy="228600"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1031" name="Check Box 7" hidden="1">
+            <xdr:cNvPr id="1047" name="Check Box 23" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1031"/>
+                  <a14:compatExt spid="_x0000_s1047"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7810F008-DDC2-41BF-A9C1-7C25E30FF607}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EDD969C-F1EE-4947-B754-75282D8A4D90}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -884,7 +950,7 @@
                   <a:latin typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
-                <a:t>valve 1</a:t>
+                <a:t>sensor 2</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -898,21 +964,21 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>4</xdr:col>
+          <xdr:col>2</xdr:col>
           <xdr:colOff>68580</xdr:colOff>
-          <xdr:row>17</xdr:row>
+          <xdr:row>26</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:ext cx="662940" cy="228600"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1032" name="Check Box 8" hidden="1">
+            <xdr:cNvPr id="1048" name="Check Box 24" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1032"/>
+                  <a14:compatExt spid="_x0000_s1048"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E970BEA-6B3D-4E71-8790-5E04887BDCA7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{992D9495-06AD-4478-A916-A2AF7A8FEB5D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -965,331 +1031,7 @@
                   <a:latin typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
-                <a:t>valve 2</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:oneCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>68580</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
-        </xdr:from>
-        <xdr:ext cx="662940" cy="228600"/>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1033" name="Check Box 9" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1033"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21F8B524-1AC2-417E-97EA-2A01063D5C5C}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Segoe UI"/>
-                  <a:cs typeface="Segoe UI"/>
-                </a:rPr>
-                <a:t>pump</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:oneCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>68580</xdr:colOff>
-          <xdr:row>19</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
-        </xdr:from>
-        <xdr:ext cx="662940" cy="228600"/>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1037" name="Check Box 13" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1037"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{741719EF-15E7-4B40-B6E1-9F6BFA8A88AF}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Segoe UI"/>
-                  <a:cs typeface="Segoe UI"/>
-                </a:rPr>
-                <a:t>valve 1</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:oneCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>68580</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
-        </xdr:from>
-        <xdr:ext cx="662940" cy="228600"/>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1038" name="Check Box 14" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1038"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{979E573E-EDD3-46BC-B970-F1BBD03CFC2E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Segoe UI"/>
-                  <a:cs typeface="Segoe UI"/>
-                </a:rPr>
-                <a:t>valve 2</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:oneCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>68580</xdr:colOff>
-          <xdr:row>21</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
-        </xdr:from>
-        <xdr:ext cx="662940" cy="228600"/>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1039" name="Check Box 15" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1039"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38DEEE88-673D-49CB-A168-1E74C688A47D}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Segoe UI"/>
-                  <a:cs typeface="Segoe UI"/>
-                </a:rPr>
-                <a:t>pump</a:t>
+                <a:t>sensor 1</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -1599,18 +1341,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB799F4-BFB2-4C5A-9DF8-C97B357196FD}">
-  <dimension ref="B5:H27"/>
+  <dimension ref="A5:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18:G23"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" style="2" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="3"/>
     <col min="6" max="6" width="8.88671875" style="2"/>
     <col min="7" max="7" width="34.33203125" style="2" customWidth="1"/>
@@ -1618,25 +1360,34 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1646,141 +1397,271 @@
       <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
+      <c r="D9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" s="15" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="17"/>
+    </row>
+    <row r="14" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="17"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="2">
+        <v>45</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="C26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="C27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C29" s="4"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="2">
+        <v>2</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B42" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B44" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="2">
+        <v>10</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B46" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="2">
+        <v>500</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B48" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="2">
-        <v>50</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="2">
-        <v>52</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="2">
-        <v>50</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B49" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="2">
-        <v>52</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="G18" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="13"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C19" s="8"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="8"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C20" s="8"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="8"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="13"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="13"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C22" s="8"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="8"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="13"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C23" s="8"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="8"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="13"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="10"/>
+      <c r="F49" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="G18:G23"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="G23:G28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1791,19 +1672,19 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId4" name="Check Box 1">
+            <control shapeId="1040" r:id="rId4" name="Check Box 16">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>68580</xdr:colOff>
-                    <xdr:row>16</xdr:row>
+                    <xdr:row>22</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>731520</xdr:colOff>
-                    <xdr:row>18</xdr:row>
+                    <xdr:row>24</xdr:row>
                     <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
@@ -1813,19 +1694,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId5" name="Check Box 2">
+            <control shapeId="1041" r:id="rId5" name="Check Box 17">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>68580</xdr:colOff>
-                    <xdr:row>17</xdr:row>
+                    <xdr:row>23</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>731520</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>25</xdr:row>
                     <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
@@ -1835,19 +1716,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1027" r:id="rId6" name="Check Box 3">
+            <control shapeId="1042" r:id="rId6" name="Check Box 18">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>68580</xdr:colOff>
-                    <xdr:row>18</xdr:row>
+                    <xdr:row>24</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>731520</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>26</xdr:row>
                     <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
@@ -1857,19 +1738,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1028" r:id="rId7" name="Check Box 4">
+            <control shapeId="1043" r:id="rId7" name="Check Box 19">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>2</xdr:col>
+                    <xdr:col>4</xdr:col>
                     <xdr:colOff>68580</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>22</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>731520</xdr:colOff>
-                    <xdr:row>21</xdr:row>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>121920</xdr:colOff>
+                    <xdr:row>24</xdr:row>
                     <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
@@ -1879,19 +1760,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1029" r:id="rId8" name="Check Box 5">
+            <control shapeId="1044" r:id="rId8" name="Check Box 20">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>2</xdr:col>
+                    <xdr:col>4</xdr:col>
                     <xdr:colOff>68580</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>23</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>731520</xdr:colOff>
-                    <xdr:row>22</xdr:row>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>121920</xdr:colOff>
+                    <xdr:row>25</xdr:row>
                     <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
@@ -1901,19 +1782,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1030" r:id="rId9" name="Check Box 6">
+            <control shapeId="1045" r:id="rId9" name="Check Box 21">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>2</xdr:col>
+                    <xdr:col>4</xdr:col>
                     <xdr:colOff>68580</xdr:colOff>
-                    <xdr:row>21</xdr:row>
+                    <xdr:row>24</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>731520</xdr:colOff>
-                    <xdr:row>23</xdr:row>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>121920</xdr:colOff>
+                    <xdr:row>26</xdr:row>
                     <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
@@ -1923,19 +1804,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1031" r:id="rId10" name="Check Box 7">
+            <control shapeId="1047" r:id="rId10" name="Check Box 23">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>4</xdr:col>
+                    <xdr:col>2</xdr:col>
                     <xdr:colOff>68580</xdr:colOff>
-                    <xdr:row>16</xdr:row>
+                    <xdr:row>27</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>121920</xdr:colOff>
-                    <xdr:row>18</xdr:row>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>731520</xdr:colOff>
+                    <xdr:row>29</xdr:row>
                     <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
@@ -1945,107 +1826,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1032" r:id="rId11" name="Check Box 8">
+            <control shapeId="1048" r:id="rId11" name="Check Box 24">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>4</xdr:col>
+                    <xdr:col>2</xdr:col>
                     <xdr:colOff>68580</xdr:colOff>
-                    <xdr:row>17</xdr:row>
+                    <xdr:row>26</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>121920</xdr:colOff>
-                    <xdr:row>19</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1033" r:id="rId12" name="Check Box 9">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>68580</xdr:colOff>
-                    <xdr:row>18</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>121920</xdr:colOff>
-                    <xdr:row>20</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1037" r:id="rId13" name="Check Box 13">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>68580</xdr:colOff>
-                    <xdr:row>19</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>121920</xdr:colOff>
-                    <xdr:row>21</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1038" r:id="rId14" name="Check Box 14">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>68580</xdr:colOff>
-                    <xdr:row>20</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>121920</xdr:colOff>
-                    <xdr:row>22</xdr:row>
-                    <xdr:rowOff>15240</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1039" r:id="rId15" name="Check Box 15">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>68580</xdr:colOff>
-                    <xdr:row>21</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>121920</xdr:colOff>
-                    <xdr:row>23</xdr:row>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>731520</xdr:colOff>
+                    <xdr:row>28</xdr:row>
                     <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>

</xml_diff>